<commit_message>
made few changes in keyword approach
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\KeywordDrivenPlusCucumberBDD\Seleniumwithjava\src\test\resources\FeatureExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DEEEB8-2045-428E-ABC1-F2F6604E2D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9AEA91-0F43-4C41-9676-5E02E60F7EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,30 +45,9 @@
     <t>General Info</t>
   </si>
   <si>
-    <t>Navigate to "Testzen Labs Form"</t>
-  </si>
-  <si>
     <t>https://testzenlabs.ie/general-information-form/</t>
   </si>
   <si>
-    <t>Enter "First Name"</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Enter "Last Name"</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Select "Country" from dropdown</t>
-  </si>
-  <si>
-    <t>Upload "Resume"</t>
-  </si>
-  <si>
     <t>//input[@placeholder='Your Name']</t>
   </si>
   <si>
@@ -90,19 +69,201 @@
     <t>//input[@type='file']</t>
   </si>
   <si>
-    <t xml:space="preserve">check the "Male" </t>
-  </si>
-  <si>
     <t>//input[@value = 'Manual Tester']</t>
   </si>
   <si>
-    <t>before Select Enter "Phone Number"</t>
-  </si>
-  <si>
     <t>//input[@placeholder = 'Your Pin Code']</t>
   </si>
   <si>
-    <t>generate a random number for pin code</t>
+    <t>Madan</t>
+  </si>
+  <si>
+    <t>Reddy</t>
+  </si>
+  <si>
+    <r>
+      <t>While filling the form, navigate to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Testzen Labs Form" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to proceed with registration.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Please ensure you correctly enter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "First Name" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>before moving to the next field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>You should carefully enter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Last Name" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>so that it matches your official documents.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Before proceeding further, make sure to enter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Phone Number" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to receive OTP verification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>In the form, select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Country" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from the dropdown list to specify your nationality.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>To complete your application, kindly upload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Resume" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in the specified format.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For gender identification, check the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Male" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>option if applicable.</t>
+    </r>
+  </si>
+  <si>
+    <t>To enhance security, generate a random number for the pin code before submission.</t>
   </si>
 </sst>
 </file>
@@ -160,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -183,6 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -467,14 +629,14 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.77734375" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="85.21875" customWidth="1"/>
     <col min="4" max="5" width="61.88671875" customWidth="1"/>
     <col min="6" max="6" width="42" style="7" customWidth="1"/>
   </cols>
@@ -493,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -506,13 +668,13 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -522,15 +684,15 @@
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+      <c r="C3" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -540,15 +702,15 @@
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -558,11 +720,11 @@
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="5">
@@ -576,14 +738,14 @@
       <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -594,11 +756,11 @@
       <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
@@ -610,27 +772,27 @@
       <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
+      <c r="C8" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="28.8">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a code related to feature creating steps
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9AEA91-0F43-4C41-9676-5E02E60F7EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880EFA82-8095-438A-8203-8E46A4F28423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Input Data</t>
   </si>
   <si>
-    <t>General Info</t>
-  </si>
-  <si>
     <t>https://testzenlabs.ie/general-information-form/</t>
   </si>
   <si>
@@ -81,8 +78,11 @@
     <t>Reddy</t>
   </si>
   <si>
-    <r>
-      <t>While filling the form, navigate to</t>
+    <t xml:space="preserve"> Fill out the General Information Form</t>
+  </si>
+  <si>
+    <r>
+      <t>Given While filling the form, navigate to</t>
     </r>
     <r>
       <rPr>
@@ -108,7 +108,7 @@
   </si>
   <si>
     <r>
-      <t>Please ensure you correctly enter</t>
+      <t>When Please ensure you correctly enter</t>
     </r>
     <r>
       <rPr>
@@ -134,7 +134,7 @@
   </si>
   <si>
     <r>
-      <t>You should carefully enter</t>
+      <t>And You should carefully enter</t>
     </r>
     <r>
       <rPr>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <r>
-      <t>Before proceeding further, make sure to enter</t>
+      <t>And Before proceeding further, make sure to enter</t>
     </r>
     <r>
       <rPr>
@@ -186,7 +186,7 @@
   </si>
   <si>
     <r>
-      <t>In the form, select</t>
+      <t>Then In the form, select</t>
     </r>
     <r>
       <rPr>
@@ -212,7 +212,7 @@
   </si>
   <si>
     <r>
-      <t>To complete your application, kindly upload</t>
+      <t>And To complete your application, kindly upload</t>
     </r>
     <r>
       <rPr>
@@ -238,7 +238,7 @@
   </si>
   <si>
     <r>
-      <t>For gender identification, check the</t>
+      <t>Then For gender identification, check the</t>
     </r>
     <r>
       <rPr>
@@ -263,7 +263,7 @@
     </r>
   </si>
   <si>
-    <t>To enhance security, generate a random number for the pin code before submission.</t>
+    <t>And To enhance security, generate a random number for the pin code before submission.</t>
   </si>
 </sst>
 </file>
@@ -629,12 +629,12 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="3" width="85.21875" customWidth="1"/>
     <col min="4" max="5" width="61.88671875" customWidth="1"/>
@@ -655,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -674,12 +674,12 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -688,16 +688,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -706,16 +706,16 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -724,7 +724,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="5">
@@ -733,7 +733,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -742,16 +742,16 @@
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -760,14 +760,14 @@
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -776,14 +776,14 @@
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="28.8">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>6</v>
@@ -792,7 +792,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keyword spell mistakes are considered by the code
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF29595-E9A4-42E5-B265-5307147FA67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3215D042-0F14-47F7-8A38-51BD593099FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,28 +81,28 @@
     <t xml:space="preserve"> Fill out the General Information Form</t>
   </si>
   <si>
-    <t>And generate a random number for the pin code before submission.</t>
-  </si>
-  <si>
-    <t>And You should carefully enter "Last Name" so that it matches your official documents.</t>
-  </si>
-  <si>
-    <t>And Before proceeding further, make sure to enter "Phone Number" to receive OTP verification.</t>
-  </si>
-  <si>
-    <t>Then In the form, select "Country" from the dropdown list to specify your nationality.</t>
-  </si>
-  <si>
     <t>And To complete your application, kindly upload "Resume" in the specified format.</t>
   </si>
   <si>
-    <t>Then check the "Male" option if applicable.</t>
-  </si>
-  <si>
-    <t>When you correctly enter "First Name" before moving to the next field.</t>
-  </si>
-  <si>
-    <t>Given  While 1 filling the form, navigate to "Testzen Labs Form" to proceed with registration.</t>
+    <t>Given  While 1 filling the form, navigation for "Testzen Labs Form" to proceed with registration.</t>
+  </si>
+  <si>
+    <t>When you correctly entered   the "First Name" before moving to the next field.</t>
+  </si>
+  <si>
+    <t>Then In the form, selection "Country" from the dropdown list to specify your nationality.</t>
+  </si>
+  <si>
+    <t>Then checked the "Male" option if applicable.</t>
+  </si>
+  <si>
+    <t>And generation a random number for the pin code before submission.</t>
+  </si>
+  <si>
+    <t>And Before proceeding further, make sure to entterring the "Phone Number" to receive OTP verification.</t>
+  </si>
+  <si>
+    <t>And You should carefully  entterred the "Last Name" so that it matches your official documents.</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -508,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -542,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -596,7 +596,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -612,7 +612,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
removed test case 2 step def
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03698781-789D-40B1-9DAF-267BEA16C8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D56120-8889-4F48-9816-B6BFF4179688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     <t>And Before proceeding further, make sure to entterring the "Phone Number" to receive OTP verification.</t>
   </si>
   <si>
-    <t>And You should carefully  entterred the "Last Name" so that it matches your official documents.</t>
+    <t>And You should carefully entterred  the "Last Name" so that it matches  your official documents.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added the step def and feature file code to convert the normal steps to bdd
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77B1EC-3802-41C3-87BD-F7CCA16CD1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA20E94-4234-4DE4-AC4C-AAA5FEDF8EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>Scenario</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>//div[contains(text(),'Africa')]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Upload "Resume" in the specified format.</t>
   </si>
 </sst>
 </file>
@@ -549,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC24C72E-6665-4A60-BD14-22FE8D88051D}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F0A23A-BBAA-4533-8152-3627A274CE8F}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -955,7 +958,20 @@
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="9"/>
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="9"/>

</xml_diff>

<commit_message>
added the tag taking from the enum
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA20E94-4234-4DE4-AC4C-AAA5FEDF8EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77930350-34D9-4416-9841-9609F1073414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Scenario</t>
   </si>
@@ -112,63 +112,21 @@
     <t>mohan</t>
   </si>
   <si>
-    <t>//input[@placeholder='Your Middle Name']</t>
-  </si>
-  <si>
     <t>reddy</t>
   </si>
   <si>
     <t>dublin</t>
   </si>
   <si>
-    <t>//input[@placeholder='Your Address']</t>
-  </si>
-  <si>
     <t>ireland</t>
   </si>
   <si>
-    <t>//input[@placeholder='Your Address Two']</t>
-  </si>
-  <si>
-    <t>//input[@placeholder='Your Pin Code']</t>
-  </si>
-  <si>
-    <t>//input[@id='profession-0']</t>
-  </si>
-  <si>
-    <t>//input[@id='exp-1']</t>
-  </si>
-  <si>
-    <t>//a[normalize-space()='Never Registered']</t>
-  </si>
-  <si>
     <t>//div[@class='selectize-input items has-options not-full']</t>
   </si>
   <si>
     <t>navigate for "Testzen Labs Form" to proceed with registration.</t>
   </si>
   <si>
-    <t>enter "madan" into "Your Name"</t>
-  </si>
-  <si>
-    <t>enter "mohan" into "Your Middle Name"</t>
-  </si>
-  <si>
-    <t>Enter "reddy" into "Your Last Name"</t>
-  </si>
-  <si>
-    <t>Enter "08999999" into "Phone Number"</t>
-  </si>
-  <si>
-    <t>Enter "dublin" into "Your Address"</t>
-  </si>
-  <si>
-    <t>Enter "ireland" into "Your Address Two"</t>
-  </si>
-  <si>
-    <t>Enter "12344" into "Your Pin Code"</t>
-  </si>
-  <si>
     <t>Click on "profession"</t>
   </si>
   <si>
@@ -178,13 +136,34 @@
     <t>select on "AsiaEuropeAfricaAustraliaSouth AmericaNorth AmericaAntarctica"</t>
   </si>
   <si>
-    <t>Click on "Never Registered"</t>
-  </si>
-  <si>
     <t>//div[contains(text(),'Africa')]</t>
   </si>
   <si>
     <t xml:space="preserve"> Upload "Resume" in the specified format.</t>
+  </si>
+  <si>
+    <t>Enter reddy into "Your Last Name"</t>
+  </si>
+  <si>
+    <t>Enter 08999999 into "Phone Number"</t>
+  </si>
+  <si>
+    <t>Enter dublin into "Your Address"</t>
+  </si>
+  <si>
+    <t>Enter ireland into "Your Address Two"</t>
+  </si>
+  <si>
+    <t>Enter 12344 into "Your Pin Code"</t>
+  </si>
+  <si>
+    <t>Enter madan into "Your Name"</t>
+  </si>
+  <si>
+    <t>Enter mohan into "Your Middle Name"</t>
+  </si>
+  <si>
+    <t>click on "Never Registered"</t>
   </si>
 </sst>
 </file>
@@ -553,7 +532,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -728,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F0A23A-BBAA-4533-8152-3627A274CE8F}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -739,9 +718,10 @@
     <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="74.88671875" customWidth="1"/>
     <col min="5" max="5" width="44.109375" customWidth="1"/>
+    <col min="6" max="6" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>5</v>
@@ -783,10 +763,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>26</v>
@@ -800,10 +777,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>27</v>
@@ -817,13 +791,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -834,10 +805,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="F6" s="9">
         <v>8999999</v>
@@ -851,13 +819,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -868,13 +833,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -885,10 +847,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F9" s="9">
         <v>12344</v>
@@ -902,10 +861,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="9"/>
     </row>
@@ -917,10 +873,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11" s="9"/>
     </row>
@@ -932,13 +885,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="F12" s="9"/>
     </row>
@@ -950,10 +903,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F13" s="9"/>
     </row>
@@ -965,7 +915,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
added a new code related to adding x path dyunamically
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77930350-34D9-4416-9841-9609F1073414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D54897-8A16-4EDA-9B37-02291E6066F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Scenario</t>
   </si>
@@ -106,6 +106,9 @@
     <t>Then chck the "Male" option if applicable.</t>
   </si>
   <si>
+    <t>Enter reddy into "Your Last Name"</t>
+  </si>
+  <si>
     <t>madan</t>
   </si>
   <si>
@@ -115,55 +118,49 @@
     <t>reddy</t>
   </si>
   <si>
+    <t>Enter madan into "Your Name"</t>
+  </si>
+  <si>
+    <t>Enter madan into "Your Middle Name"</t>
+  </si>
+  <si>
+    <t>Enter 089999 into "Phone Number"</t>
+  </si>
+  <si>
+    <t>Enter dublin into "Your Address"</t>
+  </si>
+  <si>
+    <t>Enter dublin into "Your Address Two"</t>
+  </si>
+  <si>
+    <t>Enter ireland into "Your Address three"</t>
+  </si>
+  <si>
+    <t>Enter 1234 into "Your Pin Code"</t>
+  </si>
+  <si>
     <t>dublin</t>
   </si>
   <si>
     <t>ireland</t>
   </si>
   <si>
-    <t>//div[@class='selectize-input items has-options not-full']</t>
-  </si>
-  <si>
-    <t>navigate for "Testzen Labs Form" to proceed with registration.</t>
-  </si>
-  <si>
     <t>Click on "profession"</t>
   </si>
   <si>
-    <t>Click on "exp"</t>
-  </si>
-  <si>
-    <t>select on "AsiaEuropeAfricaAustraliaSouth AmericaNorth AmericaAntarctica"</t>
-  </si>
-  <si>
-    <t>//div[contains(text(),'Africa')]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Upload "Resume" in the specified format.</t>
-  </si>
-  <si>
-    <t>Enter reddy into "Your Last Name"</t>
-  </si>
-  <si>
-    <t>Enter 08999999 into "Phone Number"</t>
-  </si>
-  <si>
-    <t>Enter dublin into "Your Address"</t>
-  </si>
-  <si>
-    <t>Enter ireland into "Your Address Two"</t>
-  </si>
-  <si>
-    <t>Enter 12344 into "Your Pin Code"</t>
-  </si>
-  <si>
-    <t>Enter madan into "Your Name"</t>
-  </si>
-  <si>
-    <t>Enter mohan into "Your Middle Name"</t>
-  </si>
-  <si>
-    <t>click on "Never Registered"</t>
+    <t>Click on "Never Registered"</t>
+  </si>
+  <si>
+    <t>Click on "exp-1"</t>
+  </si>
+  <si>
+    <t>pick the option Europe from the dropdown continents</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Your Middle Name']</t>
+  </si>
+  <si>
+    <t>navigate for "TestZEN.com"</t>
   </si>
 </sst>
 </file>
@@ -221,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -246,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC24C72E-6665-4A60-BD14-22FE8D88051D}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -699,16 +699,19 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{37A2E00A-7460-45F6-B157-3641EEC5A387}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F0A23A-BBAA-4533-8152-3627A274CE8F}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -749,9 +752,9 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -763,10 +766,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -777,10 +783,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -791,142 +800,112 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
       </c>
       <c r="F6" s="9">
-        <v>8999999</v>
+        <v>899999</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
-        <v>7</v>
-      </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
       <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="9">
-        <v>12344</v>
+        <v>35</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
       <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="7">
+        <v>12344</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="9"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2">
-        <v>11</v>
-      </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="9"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2">
-        <v>12</v>
-      </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2">
-        <v>13</v>
-      </c>
       <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="9"/>
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{CE70DCDA-C191-48F3-88A1-E6FC2E398250}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the dynamix x path from the feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D54897-8A16-4EDA-9B37-02291E6066F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8691F4-5D29-4EB1-B0E2-CC03C653FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -154,13 +154,13 @@
     <t>Click on "exp-1"</t>
   </si>
   <si>
+    <t>//input[@placeholder='Your Middle Name']</t>
+  </si>
+  <si>
+    <t>navigate for "TestZEN.com"</t>
+  </si>
+  <si>
     <t>pick the option Europe from the dropdown continents</t>
-  </si>
-  <si>
-    <t>//input[@placeholder='Your Middle Name']</t>
-  </si>
-  <si>
-    <t>navigate for "TestZEN.com"</t>
   </si>
 </sst>
 </file>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC24C72E-6665-4A60-BD14-22FE8D88051D}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F0A23A-BBAA-4533-8152-3627A274CE8F}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>5</v>
@@ -786,7 +786,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>28</v>
@@ -888,7 +888,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
removed the stemmer code and added more generic code
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653381A0-579E-46FC-9E65-F822A209DFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26C7C69-C527-4C34-8014-EF8D405D7357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Scenario</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Then In the form, selection "Country" from the dropdown list to specify your nationality.</t>
   </si>
   <si>
-    <t>And generation a random number for the pin code before submission.</t>
-  </si>
-  <si>
     <t>And Before proceeding further, make sure to entterring the "Phone Number" to receive OTP verification.</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>Given  While 1 filling the form, navigate for "Testzen Labs Form" to proceed with registration.</t>
   </si>
   <si>
-    <t>Then chck the "Male" option if applicable.</t>
-  </si>
-  <si>
     <t>Enter reddy into "Your Last Name"</t>
   </si>
   <si>
@@ -118,49 +112,76 @@
     <t>reddy</t>
   </si>
   <si>
+    <t>Enter madan into "Your Middle Name"</t>
+  </si>
+  <si>
+    <t>Enter 089999 into "Phone Number"</t>
+  </si>
+  <si>
+    <t>Enter dublin into "Your Address"</t>
+  </si>
+  <si>
+    <t>Enter dublin into "Your Address Two"</t>
+  </si>
+  <si>
+    <t>Enter ireland into "Your Address three"</t>
+  </si>
+  <si>
+    <t>Enter 1234 into "Your Pin Code"</t>
+  </si>
+  <si>
+    <t>dublin</t>
+  </si>
+  <si>
+    <t>ireland</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Your Middle Name']</t>
+  </si>
+  <si>
+    <t>pick the option Europe from the dropdown continents</t>
+  </si>
+  <si>
+    <t>And generate a random number for the pin code before submission.</t>
+  </si>
+  <si>
+    <t>Then check the "Male" option if applicable.</t>
+  </si>
+  <si>
+    <t>open  "TestZEN.com"</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Your Address']</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Your Address Two']</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Your Address three']</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Your Pin Code']</t>
+  </si>
+  <si>
+    <t>//input[@id='profession-0']</t>
+  </si>
+  <si>
+    <t>//input[@id='exp-1']</t>
+  </si>
+  <si>
+    <t>//a[normalize-space()='Never Registered']</t>
+  </si>
+  <si>
+    <t>checking on "profession"</t>
+  </si>
+  <si>
+    <t>checked on "exp-1"</t>
+  </si>
+  <si>
     <t>Enter madan into "Your Name"</t>
   </si>
   <si>
-    <t>Enter madan into "Your Middle Name"</t>
-  </si>
-  <si>
-    <t>Enter 089999 into "Phone Number"</t>
-  </si>
-  <si>
-    <t>Enter dublin into "Your Address"</t>
-  </si>
-  <si>
-    <t>Enter dublin into "Your Address Two"</t>
-  </si>
-  <si>
-    <t>Enter ireland into "Your Address three"</t>
-  </si>
-  <si>
-    <t>Enter 1234 into "Your Pin Code"</t>
-  </si>
-  <si>
-    <t>dublin</t>
-  </si>
-  <si>
-    <t>ireland</t>
-  </si>
-  <si>
-    <t>Click on "profession"</t>
-  </si>
-  <si>
-    <t>Click on "Never Registered"</t>
-  </si>
-  <si>
-    <t>Click on "exp-1"</t>
-  </si>
-  <si>
-    <t>//input[@placeholder='Your Middle Name']</t>
-  </si>
-  <si>
-    <t>navigate for "TestZEN.com"</t>
-  </si>
-  <si>
-    <t>pick the option Europe from the dropdown continents</t>
+    <t>clicking on "Never Registered"</t>
   </si>
 </sst>
 </file>
@@ -532,7 +553,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -572,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -606,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -624,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -660,7 +681,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -676,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -692,7 +713,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -711,7 +732,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -752,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>5</v>
@@ -766,13 +787,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -783,13 +804,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -800,13 +821,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -814,7 +835,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -828,10 +849,13 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -839,10 +863,13 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -850,10 +877,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -861,7 +891,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
       </c>
       <c r="F10" s="7">
         <v>12344</v>
@@ -872,7 +905,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -880,7 +916,10 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -888,7 +927,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -899,7 +938,10 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the `dynamic x path creator`
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Key\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Keyword\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26C7C69-C527-4C34-8014-EF8D405D7357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED58B8D2-70EC-465A-AEC4-34BC19F04E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -732,7 +732,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added scinchronisation to the stepkeyword class
</commit_message>
<xml_diff>
--- a/src/test/resources/FeatureExcelFiles/Data.xlsx
+++ b/src/test/resources/FeatureExcelFiles/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoha\OneDrive\Desktop\Keyword\KeywordDrivenFrameworkwithCucumber\src\test\resources\FeatureExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED58B8D2-70EC-465A-AEC4-34BC19F04E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9720C555-3DC3-41B6-8F9C-AC5C23C91B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>//input[@placeholder='Your Middle Name']</t>
   </si>
   <si>
-    <t>pick the option Europe from the dropdown continents</t>
-  </si>
-  <si>
     <t>And generate a random number for the pin code before submission.</t>
   </si>
   <si>
@@ -182,6 +179,9 @@
   </si>
   <si>
     <t>clicking on "Never Registered"</t>
+  </si>
+  <si>
+    <t>select the option Europe from the dropdown continents</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -713,7 +713,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -732,7 +732,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -773,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>5</v>
@@ -787,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -852,7 +852,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>34</v>
@@ -866,7 +866,7 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>34</v>
@@ -880,7 +880,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>35</v>
@@ -894,7 +894,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="7">
         <v>12344</v>
@@ -905,10 +905,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -916,10 +916,10 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -927,7 +927,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -938,10 +938,10 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>